<commit_message>
includes goal and format numer/strgin
</commit_message>
<xml_diff>
--- a/public/assets/maindata.xlsx
+++ b/public/assets/maindata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilherme\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilherme\Desktop\JnJ-LATAM-Analytics\jnj\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA6FE2AE-EED3-4C0D-B15B-6100C2DAF446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53CCE18-8E37-4A12-9761-1DBCF5154F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{59A75797-9169-4671-B780-AA10D9127D85}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{59A75797-9169-4671-B780-AA10D9127D85}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="76">
   <si>
     <t>Country</t>
   </si>
@@ -248,6 +248,9 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>Canada</t>
   </si>
 </sst>
 </file>
@@ -616,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E88CDFFB-FC59-497A-87BD-CB302618B985}">
-  <dimension ref="A1:K96"/>
+  <dimension ref="A1:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="I106" sqref="I106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3996,6 +3999,216 @@
         <v>47</v>
       </c>
     </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>74</v>
+      </c>
+      <c r="B97" t="s">
+        <v>75</v>
+      </c>
+      <c r="C97" t="s">
+        <v>23</v>
+      </c>
+      <c r="D97" t="s">
+        <v>12</v>
+      </c>
+      <c r="E97">
+        <v>238</v>
+      </c>
+      <c r="F97">
+        <v>374950</v>
+      </c>
+      <c r="G97">
+        <v>1</v>
+      </c>
+      <c r="H97" t="s">
+        <v>38</v>
+      </c>
+      <c r="I97" t="s">
+        <v>39</v>
+      </c>
+      <c r="J97" t="s">
+        <v>14</v>
+      </c>
+      <c r="K97" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>74</v>
+      </c>
+      <c r="B98" t="s">
+        <v>75</v>
+      </c>
+      <c r="C98" t="s">
+        <v>23</v>
+      </c>
+      <c r="D98" t="s">
+        <v>19</v>
+      </c>
+      <c r="E98">
+        <v>167</v>
+      </c>
+      <c r="F98">
+        <v>367114</v>
+      </c>
+      <c r="G98">
+        <v>8</v>
+      </c>
+      <c r="H98" t="s">
+        <v>40</v>
+      </c>
+      <c r="I98" t="s">
+        <v>41</v>
+      </c>
+      <c r="J98" t="s">
+        <v>14</v>
+      </c>
+      <c r="K98" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>74</v>
+      </c>
+      <c r="B99" t="s">
+        <v>75</v>
+      </c>
+      <c r="C99" t="s">
+        <v>42</v>
+      </c>
+      <c r="D99" t="s">
+        <v>12</v>
+      </c>
+      <c r="E99">
+        <v>21</v>
+      </c>
+      <c r="F99">
+        <v>38941</v>
+      </c>
+      <c r="G99">
+        <v>1</v>
+      </c>
+      <c r="H99" t="s">
+        <v>43</v>
+      </c>
+      <c r="I99" t="s">
+        <v>44</v>
+      </c>
+      <c r="J99" t="s">
+        <v>14</v>
+      </c>
+      <c r="K99" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>74</v>
+      </c>
+      <c r="B100" t="s">
+        <v>75</v>
+      </c>
+      <c r="C100" t="s">
+        <v>42</v>
+      </c>
+      <c r="D100" t="s">
+        <v>19</v>
+      </c>
+      <c r="E100">
+        <v>49</v>
+      </c>
+      <c r="F100">
+        <v>100906</v>
+      </c>
+      <c r="G100">
+        <v>1</v>
+      </c>
+      <c r="H100" t="s">
+        <v>45</v>
+      </c>
+      <c r="I100" t="s">
+        <v>46</v>
+      </c>
+      <c r="J100" t="s">
+        <v>14</v>
+      </c>
+      <c r="K100" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>74</v>
+      </c>
+      <c r="B101" t="s">
+        <v>75</v>
+      </c>
+      <c r="C101" t="s">
+        <v>28</v>
+      </c>
+      <c r="D101" t="s">
+        <v>12</v>
+      </c>
+      <c r="E101">
+        <v>24</v>
+      </c>
+      <c r="F101">
+        <v>31814</v>
+      </c>
+      <c r="G101">
+        <v>0</v>
+      </c>
+      <c r="H101" t="s">
+        <v>13</v>
+      </c>
+      <c r="I101" t="s">
+        <v>13</v>
+      </c>
+      <c r="J101" t="s">
+        <v>14</v>
+      </c>
+      <c r="K101" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>74</v>
+      </c>
+      <c r="B102" t="s">
+        <v>75</v>
+      </c>
+      <c r="C102" t="s">
+        <v>28</v>
+      </c>
+      <c r="D102" t="s">
+        <v>19</v>
+      </c>
+      <c r="E102">
+        <v>44</v>
+      </c>
+      <c r="F102">
+        <v>87030</v>
+      </c>
+      <c r="G102">
+        <v>1</v>
+      </c>
+      <c r="H102" t="s">
+        <v>47</v>
+      </c>
+      <c r="I102" t="s">
+        <v>48</v>
+      </c>
+      <c r="J102" t="s">
+        <v>14</v>
+      </c>
+      <c r="K102" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="B1:K79" xr:uid="{E88CDFFB-FC59-497A-87BD-CB302618B985}"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>

</xml_diff>